<commit_message>
Update L1: Average earning in agricultural production / average earning in manufacturing
</commit_message>
<xml_diff>
--- a/01_Input/05_ResourcePressureAssessment_DataPreparation.xlsx
+++ b/01_Input/05_ResourcePressureAssessment_DataPreparation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Branches\WEFN\01_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B353ECC0-03F5-4038-BA53-22E03D2B5039}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC8F1E9-3F3C-48D9-AFB3-D46BAF8D7314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="140">
   <si>
     <t>總用水量/再生水資源</t>
   </si>
@@ -101,9 +101,6 @@
   </si>
   <si>
     <t>https://agrstat.coa.gov.tw/sdweb/public/book/Book.aspx</t>
-  </si>
-  <si>
-    <t>https://statdb.dgbas.gov.tw/pxweb/Dialog/Saveshow.asp</t>
   </si>
   <si>
     <t>https://statview.coa.gov.tw/aqsys_on/importantArgiGoal_lv3_1_6_3_1.html</t>
@@ -401,69 +398,6 @@
   <si>
     <t>Share of monitoring sites in agricultural areas that exceed recommended drinking water limits for nitrates, phosphorus and pesticides in surface water and groundwater</t>
     <phoneticPr fontId="11" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>製造業平均收入</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>/</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>農業生產平均收入</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>農業生產平均收入</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>5</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="major"/>
-      </rPr>
-      <t>農家所得</t>
-    </r>
   </si>
   <si>
     <r>
@@ -876,11 +810,108 @@
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>每人每月總薪資製造業</t>
+    <t>L1.1</t>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
   <si>
-    <t>製造業平均收入</t>
+    <t>L1.2</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average earning in agricultural production</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>Average earning in manufacturing</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1=L1.1/L1.2</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1.1</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>L1.2</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>農業統計年報 -&gt;  五、農家與農家經濟 -&gt; 3農家所得 (Assume 3.3 person in a family)</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://www.stat.gov.tw/ct.asp?xItem=47229&amp;ctNode=526</t>
+    <phoneticPr fontId="11" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>109</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>年薪資與生產力統計年報</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>表７歷年各業受僱員工每人每月總薪資</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> -&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="136"/>
+        <scheme val="major"/>
+      </rPr>
+      <t>製造業</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="major"/>
+      </rPr>
+      <t xml:space="preserve"> Manufacturing</t>
+    </r>
     <phoneticPr fontId="11" type="noConversion"/>
   </si>
 </sst>
@@ -897,7 +928,7 @@
     <numFmt numFmtId="182" formatCode="#,##0.0000"/>
     <numFmt numFmtId="184" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="33">
+  <fonts count="32">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1115,14 +1146,6 @@
       <charset val="136"/>
       <scheme val="major"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="3"/>
-      <charset val="136"/>
-      <scheme val="major"/>
-    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -1181,7 +1204,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="3" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1354,11 +1377,8 @@
     <xf numFmtId="184" fontId="20" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1577,10 +1597,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08D9907D-936E-41B8-B384-16814991858B}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="L2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="P24" sqref="P24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1591,69 +1614,77 @@
     <col min="13" max="13" width="9.7109375" style="63" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="9.140625" style="63"/>
     <col min="15" max="15" width="9.7109375" style="63" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="63"/>
+    <col min="16" max="16" width="9.140625" style="63"/>
+    <col min="17" max="18" width="8.42578125" style="63" bestFit="1" customWidth="1"/>
+    <col min="19" max="16384" width="9.140625" style="63"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="64" customFormat="1" ht="15.75">
+    <row r="1" spans="1:21" s="64" customFormat="1" ht="15.75">
       <c r="A1" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B1" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="64" t="s">
+        <v>94</v>
+      </c>
+      <c r="D1" s="64" t="s">
+        <v>95</v>
+      </c>
+      <c r="E1" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="64" t="s">
-        <v>98</v>
-      </c>
-      <c r="D1" s="64" t="s">
-        <v>99</v>
-      </c>
-      <c r="E1" s="64" t="s">
+      <c r="F1" s="64" t="s">
+        <v>102</v>
+      </c>
+      <c r="G1" s="64" t="s">
+        <v>106</v>
+      </c>
+      <c r="H1" s="64" t="s">
         <v>61</v>
       </c>
-      <c r="F1" s="64" t="s">
-        <v>106</v>
-      </c>
-      <c r="G1" s="64" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" s="64" t="s">
+      <c r="I1" s="64" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="J1" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="64" t="s">
+        <v>117</v>
+      </c>
+      <c r="L1" s="64" t="s">
+        <v>118</v>
+      </c>
+      <c r="M1" s="64" t="s">
         <v>63</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="N1" s="64" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" s="64" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" s="64" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="64" t="s">
-        <v>121</v>
-      </c>
-      <c r="L1" s="64" t="s">
-        <v>122</v>
-      </c>
-      <c r="M1" s="64" t="s">
+      <c r="Q1" s="64" t="s">
+        <v>135</v>
+      </c>
+      <c r="R1" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="64" t="s">
         <v>64</v>
       </c>
-      <c r="N1" s="64" t="s">
-        <v>125</v>
-      </c>
-      <c r="O1" s="64" t="s">
-        <v>126</v>
-      </c>
-      <c r="P1" s="64" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q1" s="64" t="s">
+      <c r="T1" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="64" t="s">
+      <c r="U1" s="64" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="64" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19">
+    </row>
+    <row r="2" spans="1:21">
       <c r="A2" s="63">
         <v>2012</v>
       </c>
@@ -1704,8 +1735,19 @@
       <c r="O2" s="63">
         <v>847334</v>
       </c>
-    </row>
-    <row r="3" spans="1:19">
+      <c r="P2" s="63">
+        <f>Q2/R2</f>
+        <v>0.55578386544609637</v>
+      </c>
+      <c r="Q2" s="82">
+        <f>995645/3.3/12</f>
+        <v>25142.550505050505</v>
+      </c>
+      <c r="R2" s="63">
+        <v>45238</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" s="63">
         <v>2013</v>
       </c>
@@ -1756,8 +1798,19 @@
       <c r="O3" s="63">
         <v>844097</v>
       </c>
-    </row>
-    <row r="4" spans="1:19">
+      <c r="P3" s="63">
+        <f t="shared" ref="P3:P8" si="5">Q3/R3</f>
+        <v>0.5474913396417973</v>
+      </c>
+      <c r="Q3" s="82">
+        <f>985342.5016/3.3/12</f>
+        <v>24882.386404040404</v>
+      </c>
+      <c r="R3" s="63">
+        <v>45448</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" s="63">
         <v>2014</v>
       </c>
@@ -1808,8 +1861,19 @@
       <c r="O4" s="63">
         <v>835507</v>
       </c>
-    </row>
-    <row r="5" spans="1:19">
+      <c r="P4" s="63">
+        <f t="shared" si="5"/>
+        <v>0.54956804867553422</v>
+      </c>
+      <c r="Q4" s="82">
+        <f>1023247.7843/3.3/12</f>
+        <v>25839.590512626266</v>
+      </c>
+      <c r="R4" s="63">
+        <v>47018</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" s="63">
         <v>2015</v>
       </c>
@@ -1860,8 +1924,19 @@
       <c r="O5" s="63">
         <v>833176</v>
       </c>
-    </row>
-    <row r="6" spans="1:19">
+      <c r="P5" s="63">
+        <f t="shared" si="5"/>
+        <v>0.53171591305662302</v>
+      </c>
+      <c r="Q5" s="82">
+        <f>1025698.5/3.3/12</f>
+        <v>25901.477272727276</v>
+      </c>
+      <c r="R5" s="63">
+        <v>48713</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" s="63">
         <v>2016</v>
       </c>
@@ -1912,8 +1987,19 @@
       <c r="O6" s="63">
         <v>829527</v>
       </c>
-    </row>
-    <row r="7" spans="1:19">
+      <c r="P6" s="63">
+        <f t="shared" si="5"/>
+        <v>0.55122968641296832</v>
+      </c>
+      <c r="Q6" s="82">
+        <f>1073142.3322/3.3/12</f>
+        <v>27099.553843434347</v>
+      </c>
+      <c r="R6" s="63">
+        <v>49162</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="63">
         <v>2017</v>
       </c>
@@ -1964,8 +2050,19 @@
       <c r="O7" s="63">
         <v>825947</v>
       </c>
-    </row>
-    <row r="8" spans="1:19">
+      <c r="P7" s="63">
+        <f t="shared" si="5"/>
+        <v>0.52329609405551636</v>
+      </c>
+      <c r="Q7" s="82">
+        <f>1050176.1384/3.3/12</f>
+        <v>26519.59945454546</v>
+      </c>
+      <c r="R7" s="63">
+        <v>50678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" s="63">
         <v>2018</v>
       </c>
@@ -2015,6 +2112,17 @@
       </c>
       <c r="O8" s="63">
         <v>822364</v>
+      </c>
+      <c r="P8" s="63">
+        <f t="shared" si="5"/>
+        <v>0.52430164877795093</v>
+      </c>
+      <c r="Q8" s="82">
+        <f>1099324.6585/3.3/12</f>
+        <v>27760.723699494949</v>
+      </c>
+      <c r="R8" s="63">
+        <v>52948</v>
       </c>
     </row>
   </sheetData>
@@ -2034,7 +2142,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P14" sqref="P14"/>
+      <selection pane="bottomRight" activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -2053,10 +2161,10 @@
   <sheetData>
     <row r="1" spans="1:66" s="58" customFormat="1" ht="12.75">
       <c r="A1" s="58" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C1" s="60"/>
       <c r="D1" s="61">
@@ -2276,7 +2384,7 @@
     </row>
     <row r="3" spans="1:66" ht="14.25">
       <c r="C3" s="75" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D3" s="34">
         <v>59900</v>
@@ -2384,7 +2492,7 @@
     </row>
     <row r="4" spans="1:66" ht="12.75">
       <c r="B4" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="32" t="s">
         <v>0</v>
@@ -2515,7 +2623,7 @@
     </row>
     <row r="5" spans="1:66" ht="57">
       <c r="B5" s="27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C5" s="36"/>
       <c r="D5" s="3" t="s">
@@ -2750,7 +2858,7 @@
     </row>
     <row r="7" spans="1:66" ht="28.5">
       <c r="B7" s="27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D7" s="38">
         <v>0.87629999999999997</v>
@@ -2858,7 +2966,7 @@
     </row>
     <row r="8" spans="1:66" ht="14.25">
       <c r="B8" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C8" s="36"/>
       <c r="D8" s="38">
@@ -3175,7 +3283,7 @@
     </row>
     <row r="11" spans="1:66" ht="12.75">
       <c r="B11" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C11" s="32" t="s">
         <v>10</v>
@@ -3417,7 +3525,7 @@
     </row>
     <row r="13" spans="1:66" ht="12.75">
       <c r="B13" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="32" t="s">
         <v>11</v>
@@ -3883,7 +3991,7 @@
     </row>
     <row r="17" spans="2:66" ht="12.75">
       <c r="B17" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C17" s="32" t="s">
         <v>13</v>
@@ -4014,7 +4122,7 @@
     </row>
     <row r="18" spans="2:66" ht="25.5">
       <c r="B18" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C18" s="32" t="s">
         <v>18</v>
@@ -4234,7 +4342,7 @@
     </row>
     <row r="20" spans="2:66" ht="12.75">
       <c r="B20" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C20" s="32" t="s">
         <v>17</v>
@@ -4702,7 +4810,7 @@
     </row>
     <row r="24" spans="2:66" ht="12.75">
       <c r="B24" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C24" s="32" t="s">
         <v>20</v>
@@ -4830,7 +4938,7 @@
     </row>
     <row r="25" spans="2:66" ht="28.5">
       <c r="B25" s="56" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C25" s="36"/>
       <c r="D25" s="37">
@@ -70048,10 +70156,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="12.75"/>
@@ -70059,351 +70167,351 @@
     <col min="1" max="1" width="10.28515625" style="67" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="41.28515625" style="67" customWidth="1"/>
     <col min="3" max="3" width="60.7109375" style="67" customWidth="1"/>
-    <col min="4" max="4" width="64" style="67" customWidth="1"/>
+    <col min="4" max="4" width="64.5703125" style="67" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="14.42578125" style="67"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75">
       <c r="A1" s="65" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>54</v>
-      </c>
       <c r="C1" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="66" t="s">
         <v>56</v>
-      </c>
-      <c r="D1" s="66" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="25.5">
       <c r="A2" s="67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C2" s="67" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="67" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B3" s="67" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C3" s="73" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D3" s="67" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="67" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="67" t="s">
         <v>91</v>
       </c>
-      <c r="B4" s="67" t="s">
-        <v>95</v>
-      </c>
       <c r="C4" s="73" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="67" t="s">
         <v>97</v>
-      </c>
-      <c r="D4" s="67" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="51">
       <c r="A5" s="67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" s="67" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="D5" s="67" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5">
       <c r="A6" s="67" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B6" s="67" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C6" s="73" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D6" s="80" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5">
       <c r="A7" s="67" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B7" s="67" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C7" s="78">
         <f>0.857142857142857</f>
         <v>0.85714285714285698</v>
       </c>
       <c r="D7" s="67" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5">
       <c r="A8" s="67" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" s="67" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" s="73" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5">
       <c r="A9" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B9" s="67" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C9" s="73" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5">
       <c r="A10" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10" s="67" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5">
       <c r="A11" s="67" t="s">
+        <v>110</v>
+      </c>
+      <c r="B11" s="67" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="67" t="s">
-        <v>118</v>
-      </c>
       <c r="C11" s="73" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="67" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="B12" s="67" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C12" s="73" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="67" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" s="67" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D13" s="80"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="67" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B14" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="67" t="s">
         <v>129</v>
-      </c>
-      <c r="C14" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D14" s="67" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="B15" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="D15" s="67" t="s">
         <v>128</v>
-      </c>
-      <c r="B15" s="67" t="s">
-        <v>130</v>
-      </c>
-      <c r="C15" s="73" t="s">
-        <v>124</v>
-      </c>
-      <c r="D15" s="67" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5">
       <c r="A16" s="67" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="38.25">
+        <v>82</v>
+      </c>
+      <c r="C16" s="67" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="25.5">
       <c r="A17" s="67" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
       <c r="B17" s="67" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="38.25">
+        <v>132</v>
+      </c>
+      <c r="C17" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="D17" s="80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="25.5">
       <c r="A18" s="67" t="s">
-        <v>38</v>
+        <v>131</v>
       </c>
       <c r="B18" s="67" t="s">
-        <v>88</v>
+        <v>133</v>
+      </c>
+      <c r="C18" s="73" t="s">
+        <v>138</v>
+      </c>
+      <c r="D18" s="67" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="38.25">
       <c r="A19" s="67" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B19" s="67" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="51">
-      <c r="B21" s="68" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="38.25">
+      <c r="A20" s="67" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="67" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="38.25">
+      <c r="A21" s="67" t="s">
+        <v>38</v>
+      </c>
+      <c r="B21" s="67" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="51">
+      <c r="B23" s="70" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" s="68" t="s">
         <v>70</v>
       </c>
-      <c r="C21" s="83" t="s">
-        <v>135</v>
-      </c>
-      <c r="D21" s="82" t="s">
-        <v>134</v>
-      </c>
-      <c r="E21" s="69" t="s">
+      <c r="D23" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="H21" s="68"/>
-    </row>
-    <row r="22" spans="1:8" ht="51">
-      <c r="C22" s="71" t="s">
+      <c r="E23" s="72" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="68" t="s">
         <v>71</v>
       </c>
-      <c r="D22" s="68" t="s">
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="C24" s="71" t="s">
         <v>72</v>
       </c>
-      <c r="E22" s="69" t="s">
+      <c r="D24" s="68" t="s">
+        <v>73</v>
+      </c>
+      <c r="H24" s="68"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="C25" s="68"/>
+      <c r="H25" s="68"/>
+    </row>
+    <row r="26" spans="1:8" ht="25.5">
+      <c r="B26" s="70" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" s="71" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="H22" s="68"/>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="C23" s="68"/>
-      <c r="H23" s="68"/>
-    </row>
-    <row r="24" spans="1:8" ht="51">
-      <c r="B24" s="70" t="s">
-        <v>73</v>
-      </c>
-      <c r="C24" s="68" t="s">
-        <v>74</v>
-      </c>
-      <c r="D24" s="69" t="s">
+      <c r="E26" s="68" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="25.5">
+      <c r="C27" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="E24" s="72" t="s">
-        <v>25</v>
-      </c>
-      <c r="F24" s="68" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" s="68"/>
-      <c r="H24" s="68"/>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="C25" s="71" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="68" t="s">
-        <v>77</v>
-      </c>
-      <c r="H25" s="68"/>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="C26" s="68"/>
-      <c r="H26" s="68"/>
-    </row>
-    <row r="27" spans="1:8" ht="25.5">
-      <c r="B27" s="70" t="s">
+    </row>
+    <row r="28" spans="1:8">
+      <c r="C28" s="71"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="C29" s="68"/>
+    </row>
+    <row r="30" spans="1:8" ht="25.5">
+      <c r="B30" s="70" t="s">
         <v>78</v>
       </c>
-      <c r="C27" s="71" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" s="69" t="s">
-        <v>25</v>
-      </c>
-      <c r="E27" s="68" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="25.5">
-      <c r="C28" s="68" t="s">
-        <v>81</v>
-      </c>
-      <c r="D28" s="69" t="s">
+      <c r="C30" s="69" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8">
-      <c r="C29" s="71"/>
-    </row>
-    <row r="30" spans="1:8">
-      <c r="C30" s="68"/>
-    </row>
-    <row r="31" spans="1:8" ht="25.5">
-      <c r="B31" s="70" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="69" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E21" r:id="rId1" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
-    <hyperlink ref="E22" r:id="rId2" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
-    <hyperlink ref="D24" r:id="rId3" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
-    <hyperlink ref="E24" r:id="rId4" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
-    <hyperlink ref="D27" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
-    <hyperlink ref="D28" r:id="rId6" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
-    <hyperlink ref="C31" r:id="rId7" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
-    <hyperlink ref="C3" r:id="rId8" xr:uid="{B1001F65-51C3-4C73-9F96-4F0D5F22FB4D}"/>
-    <hyperlink ref="C4" r:id="rId9" xr:uid="{E4381052-4B15-4DFD-B543-57656A2B1E70}"/>
-    <hyperlink ref="C6" r:id="rId10" xr:uid="{49805B75-8CD3-4397-92FE-0E904C803CA8}"/>
-    <hyperlink ref="C8" r:id="rId11" location="p=32" xr:uid="{275D182C-551E-42FB-B5C3-BA2A57D56231}"/>
-    <hyperlink ref="C9" r:id="rId12" location="p=32" xr:uid="{C2A27A77-81C9-4625-90A9-7E42BAD1F6FF}"/>
-    <hyperlink ref="C11" r:id="rId13" xr:uid="{2197FC4F-64D1-41A8-BACC-8F32AD6E7829}"/>
-    <hyperlink ref="C12" r:id="rId14" xr:uid="{D3D0A98D-9690-4C13-AF4C-C80FD8482A90}"/>
-    <hyperlink ref="C14" r:id="rId15" xr:uid="{DF8104B4-C2A8-4DC8-94F1-A32EAD95418B}"/>
-    <hyperlink ref="C15" r:id="rId16" xr:uid="{4E72F009-8B01-49C8-878B-C53A74D6743F}"/>
+    <hyperlink ref="D23" r:id="rId1" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="E23" r:id="rId2" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="D26" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="D27" r:id="rId4" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="C30" r:id="rId5" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="C3" r:id="rId6" xr:uid="{B1001F65-51C3-4C73-9F96-4F0D5F22FB4D}"/>
+    <hyperlink ref="C4" r:id="rId7" xr:uid="{E4381052-4B15-4DFD-B543-57656A2B1E70}"/>
+    <hyperlink ref="C6" r:id="rId8" xr:uid="{49805B75-8CD3-4397-92FE-0E904C803CA8}"/>
+    <hyperlink ref="C8" r:id="rId9" location="p=32" xr:uid="{275D182C-551E-42FB-B5C3-BA2A57D56231}"/>
+    <hyperlink ref="C9" r:id="rId10" location="p=32" xr:uid="{C2A27A77-81C9-4625-90A9-7E42BAD1F6FF}"/>
+    <hyperlink ref="C11" r:id="rId11" xr:uid="{2197FC4F-64D1-41A8-BACC-8F32AD6E7829}"/>
+    <hyperlink ref="C12" r:id="rId12" xr:uid="{D3D0A98D-9690-4C13-AF4C-C80FD8482A90}"/>
+    <hyperlink ref="C14" r:id="rId13" xr:uid="{DF8104B4-C2A8-4DC8-94F1-A32EAD95418B}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{4E72F009-8B01-49C8-878B-C53A74D6743F}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{84061280-3C73-4DFE-B619-9D3497B299A5}"/>
+    <hyperlink ref="C18" r:id="rId16" xr:uid="{2AA64D65-6A7E-4D4D-B64B-3E6CF40A4C5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -70495,7 +70603,7 @@
     </row>
     <row r="2" spans="1:66" ht="39.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B2" s="54" t="s">
         <v>0</v>
@@ -70609,7 +70717,7 @@
     </row>
     <row r="3" spans="1:66" ht="39.75" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="28" t="s">
         <v>3</v>
@@ -70723,7 +70831,7 @@
     </row>
     <row r="4" spans="1:66" ht="39.75" customHeight="1">
       <c r="A4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" s="54" t="s">
         <v>5</v>
@@ -70837,7 +70945,7 @@
     </row>
     <row r="5" spans="1:66" ht="39.75" customHeight="1">
       <c r="A5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" s="54" t="s">
         <v>6</v>
@@ -70951,7 +71059,7 @@
     </row>
     <row r="6" spans="1:66" ht="39.75" customHeight="1">
       <c r="A6" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="28" t="s">
         <v>10</v>
@@ -71064,7 +71172,7 @@
     </row>
     <row r="7" spans="1:66" ht="39.75" customHeight="1">
       <c r="A7" s="8" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B7" s="54" t="s">
         <v>11</v>
@@ -71135,7 +71243,7 @@
     </row>
     <row r="8" spans="1:66" ht="39.75" customHeight="1">
       <c r="A8" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B8" s="53" t="s">
         <v>13</v>
@@ -71207,7 +71315,7 @@
     </row>
     <row r="9" spans="1:66" ht="39.75" customHeight="1">
       <c r="A9" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="55" t="s">
         <v>17</v>
@@ -71278,7 +71386,7 @@
     </row>
     <row r="10" spans="1:66" ht="39.75" customHeight="1">
       <c r="A10" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="53" t="s">
         <v>20</v>
@@ -71350,7 +71458,7 @@
     </row>
     <row r="11" spans="1:66" ht="39.75" customHeight="1">
       <c r="A11" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B11" s="53" t="s">
         <v>24</v>

</xml_diff>